<commit_message>
se suben los scripts y documentos necesarios - grupo 7
</commit_message>
<xml_diff>
--- a/Grupo07/docs/income_dictionary.xlsx
+++ b/Grupo07/docs/income_dictionary.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9cb947233478d2b5/Documentos/_IA/202601_ml_pucp_pregrado/trabajos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leydi\Documents\Machine-Learning-para-Finanzas_2026_0\Grupo07\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{375FF363-18C1-4ABC-A8EE-8B7B4F32CA5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4DA2A1C-52A9-4458-A4B1-9ABDB4DAA698}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3FF69D-8E7C-4AD1-AC60-0AC130FE92E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54952E9C-228E-4F9B-929C-B363D3D5F4DE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{54952E9C-228E-4F9B-929C-B363D3D5F4DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -583,14 +584,14 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="25.25" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="32.6328125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -618,7 +619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -632,7 +633,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -646,7 +647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -660,7 +661,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -674,7 +675,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -688,7 +689,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -702,7 +703,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -716,7 +717,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -730,7 +731,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -744,7 +745,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -758,7 +759,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -772,7 +773,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -786,7 +787,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>

</xml_diff>